<commit_message>
routes (for excel form) creating from database READY
</commit_message>
<xml_diff>
--- a/downloads/ds.xlsx
+++ b/downloads/ds.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="231">
   <si>
     <t xml:space="preserve">მარშრუტის. № </t>
   </si>
@@ -390,14 +390,6 @@
     <t>სოფელი გლდანი</t>
   </si>
   <si>
-    <t>სოფელ გლდანი (ბორის პაიჭაძის ქ. #18 სახლის მიმდებარედ) - სოფელი გლდანი (ბორის პაიჭაძის ქ. - ვიტალი დარასელიას ქ. - ვახტანგ გორგასალის ქ. – 26 მაისის ქ.).   - ლიბანის შესახვევი - ლიბანის ქუჩა - იპოლიტე-ივანოვის ქუჩა ქერჩის ქუჩა - აკაკი ვასაძის ქუჩა - ომარ ხიხანიშვილის ქ. - მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია).
-უკუ მიმართულებით: მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია) - ილია ვეკუას ქ.  - აკაკი ვასაძის ქ. - შემდეგ იგივე სქემით.</t>
-  </si>
-  <si>
-    <t>სოფელ გლდანი (26 მაისის ქ. #83- 26 მაისის ქუჩა).   - ლიბანის შესახვევი - ლიბანის ქუჩა - იპოლიტე-ივანოვის ქუჩა -  ქერჩის ქუჩა - აკაკი ვასაძის ქუჩა - ომარ ხიხანიშვილის ქ. - მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია).
-უკუ მიმართულებით: მ/ს 'ახმეტელის თეატრი' (მიმდებარე ტერიტორია) - ილია ვეკუას ქ. - აკაკი ვასაძის ქ. - შემდეგ იგივე სქემით.</t>
-  </si>
-  <si>
     <t xml:space="preserve">აკაკი ბელიაშვილის ქ. (#40-ის მიმდებარედ) - აკაკი ბელიაშვილის ქ. - სანდრო ახმეტელის ქ - რობერტ ბარძიმაშვილის ქ. - პაიჭაძის ქ. (მობრუნება პაიჭაძის ქ. #5'ა'-სთან) - ევგენი მიქელაძის ქ. - აკაკი ბელიაშვილის ქ. - აკაკი ბაქრაძის ქ. - გრიგოლ რობაქიძის გამზირი - შალიკაშვილის ხიდი - აკაკი წერეთლის გამზირი - გიორგი ცაბაძის ქ. - დავით აღმაშენებლის გამზირი - თამარ მეფის გამზირი - გმირთა მოედანი - ვარაზისხევის ქ. - პეტრე მელიქიშვილის ქ. - მერაბ კოსტავას ქ. - შოთა რუსთაველის გამზირი - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. - ნიკოლოზ ბარათაშვილის ქ. - ნიკოლოზ ბარათაშვილის ხიდი - ნიკოლოზ ბარათაშვილის აღმართი - მ/ს ,,ავლაბარი' (მიმდებარედ).
 უკუმიმართულებით: მ/ს ,,ავლაბარი' (მიმდებარედ) - ნიკოლოზ ბარათაშვილის აღმართი - ნიკოლოზ ბარათაშვილის ხიდი - მარჯვენა სანაპირო - მიხეილ ჯავახიშვილის ქუჩა - რუსთაველის გამზირი - მერაბ კოსტავას ქ. - გმირთა მოედანი - თამარ მეფის გამზირი - მიხეილ წინამძღვრიშვილის ქ. - აკაკი წერეთლის გამზირი - შალიკაშვილის ხიდი  - აკაკი ბელიაშვილის ქ. (მობრუნება ჯორჯ ბალანჩინის ქუჩაზე, 'Mcdonald's'-ის მიმდებარედ) - აკაკი ბელიაშვილის ქ. (#40-ის მიმდებარედ).
 </t>
@@ -665,13 +657,6 @@
     <t>ნუცუბიძის V მ/რ</t>
   </si>
   <si>
-    <t>საქართველოს სასჯელაღსრულების, პრობაციისა და იურიდიული დახმარების საკითხთა სამინისტროს სასჯელაღსრულების დეპარტამეტის დაქვემდებარებაში არსებული N6 დაწესებულება - სოფელი კრწანისი - კრწანისის სასწავლო ცენტრი - შსს-ოს აგარაკები - გიგანტის დასახლება - ზოოვეტერინარული ინსტიტუტის დასახლება - სოფ. სოღანლუღი - ქვემო ფონიჭალის დასახლება - რუსთავის გზატკეცილი - გორგასლის ქ. - მეტეხის ხიდი - რიყე - მარცხენა სანაპირო - ბარათაშვილის ქ. (მობრუნება ბარათაშვილისა და პუშკინის ქუჩების გადაკვეთასთან, გაჩერება 'კონკის' მხარეს)
-უკუ მიმართულებით: ბარათაშვილის ქ. ('კონკის' მხარეს) - მარჯვენა სანაპირო - გორგასალის ქ. - შემდეგ იგივე სქემით</t>
-  </si>
-  <si>
-    <t>№6-ე სასჯელ-აღსრულების დაწესებულება</t>
-  </si>
-  <si>
     <t xml:space="preserve">სოფელი ტაბახმელა (#7 და #6 სახლების გზაგამყოფის მიმდებარედ ) - თბილისი-კოჯრის ქ. (სოფ. შინდისის, სოფელი წავკისის, წავკისის ველის გავლით) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი - ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ).                                             უკუმიმართულებით: ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – მიხეილ ლერმონტოვის ქ. - პაოლო იაშვილის ქ. - ამაღლების ქ. -  მარო მაყაშვილის ქ. - მარო მაყაშვილის აღმართი - კოჯრის გზატკეცილი - თბილისი-კოჯრის ქ. ( წავკისის ველის, სოფელი წავკისის, სოფ. შინდისის გავლით) - სოფელი ტაბახმელა (კვირაცხოვლის ქ. - საცხოვრებელი კორპუსი - იაშაღაშვილის ქ. - #7,11,12,13,14 სახლი - #6,5,4,3,2,1 სახლი - #7 და #6 სახლების გზაგამყოფის მიმდებარედ). </t>
   </si>
   <si>
@@ -682,6 +667,13 @@
   </si>
   <si>
     <t>სოფელი დიღომი</t>
+  </si>
+  <si>
+    <t>დაბა კიკეთი - თბილისი-კოჯრის გზა (სოფ. დიდება, დაბა კოჯორი, სოფ. ტაბახმელა, სოფ. შინდისი, სოფ. წავკისი, წავკისის ველის გავლით) - კოჯრის გზატკეცილი - მარო მაყაშვილის აღმართი - მარო მაყაშვილის ქ. - ამაღლების ქ. - ლადო ასათიანის შესახვევი - ლადო ასათიანის ქ. - შალვა დადიანის ქ. - თავისუფლების მოედანი -ალექსანდრე პუშკინის ქ. – ნიკოლოზ ბარათაშვილის ქ. – ნიკოლოზ ბარათაშვილის ხიდი – მარცხენა სანაპირო – ნიკოლოზ ბარათაშვილის ხიდი – ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ)
+უკუმიმართულებით:  ნიკოლოზ ბარათაშვილის ქ. (№2-ის მიმდებარედ) – ალექსანდრე პუშკინის ქ. – თავისუფლების მოედანი – გიორგი ლეონიძის ქ. – მიხეილ ლერმონტოვის ქ. – პაოლო იაშვილის ქ. – ამაღლების ქ. – მარო მაყაშვილის ქ. – მარო მაყაშვილის აღმართი – კოჯრის გზატკეცილი – შემდეგ არსებული სქემით.</t>
+  </si>
+  <si>
+    <t>კიკეთი</t>
   </si>
   <si>
     <t>სოფ. ლისი - სოფ. თხინვალი - ახალი იპოდრომი -  ნუცუბიძის IV-II მ/რ - ჟღენტის ქ. - ნუცუბიძის ქ. - თავაძის ქ. - ზაქარიაძის ქ. - ვაჟა ფშაველას ჩიხი - მ/ს 'დელისი' (მიმდებარედ) 
@@ -2638,6 +2630,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s" s="3">
+        <f>SUM(F5:F114)</f>
         <v>5</v>
       </c>
       <c r="G1" t="s" s="1">
@@ -5457,9 +5450,7 @@
       <c r="B46" t="n" s="6">
         <v>3.0</v>
       </c>
-      <c r="C46" t="s" s="6">
-        <v>114</v>
-      </c>
+      <c r="C46" s="6"/>
       <c r="D46" t="s" s="6">
         <v>21</v>
       </c>
@@ -5493,9 +5484,7 @@
       <c r="N46" t="n" s="11">
         <v>0.96875</v>
       </c>
-      <c r="O46" t="s" s="9">
-        <v>28</v>
-      </c>
+      <c r="O46" s="9"/>
       <c r="P46" t="n" s="11">
         <v>0.9027777777777778</v>
       </c>
@@ -5520,9 +5509,7 @@
       <c r="B47" t="n" s="6">
         <v>3.0</v>
       </c>
-      <c r="C47" t="s" s="6">
-        <v>115</v>
-      </c>
+      <c r="C47" s="6"/>
       <c r="D47" t="s" s="6">
         <v>21</v>
       </c>
@@ -5556,9 +5543,7 @@
       <c r="N47" t="n" s="11">
         <v>0.9791666666666666</v>
       </c>
-      <c r="O47" t="s" s="9">
-        <v>28</v>
-      </c>
+      <c r="O47" s="9"/>
       <c r="P47" t="n" s="11">
         <v>0.9305555555555556</v>
       </c>
@@ -5584,7 +5569,7 @@
         <v>2.0</v>
       </c>
       <c r="C48" t="s" s="6">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D48" t="s" s="6">
         <v>21</v>
@@ -5620,7 +5605,7 @@
         <v>1.0097222222222222</v>
       </c>
       <c r="O48" t="s" s="9">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="P48" t="n" s="11">
         <v>0.9027777777777778</v>
@@ -5629,7 +5614,7 @@
         <v>0.9472222222222222</v>
       </c>
       <c r="R48" t="s" s="9">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="S48" t="n" s="11">
         <v>0.9243055555555556</v>
@@ -5649,7 +5634,7 @@
         <v>3.0</v>
       </c>
       <c r="C49" t="s" s="6">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D49" t="s" s="6">
         <v>21</v>
@@ -5685,7 +5670,7 @@
         <v>0.9875</v>
       </c>
       <c r="O49" t="s" s="9">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="P49" t="n" s="11">
         <v>0.9027777777777778</v>
@@ -5714,7 +5699,7 @@
         <v>3.0</v>
       </c>
       <c r="C50" t="s" s="6">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D50" t="s" s="6">
         <v>21</v>
@@ -5750,7 +5735,7 @@
         <v>0.9909722222222223</v>
       </c>
       <c r="O50" t="s" s="9">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="P50" t="n" s="11">
         <v>0.9263888888888889</v>
@@ -5779,7 +5764,7 @@
         <v>1.0</v>
       </c>
       <c r="C51" t="s" s="6">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D51" t="s" s="6">
         <v>21</v>
@@ -5815,7 +5800,7 @@
         <v>0.9951388888888889</v>
       </c>
       <c r="O51" t="s" s="9">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="P51" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -5844,7 +5829,7 @@
         <v>2.0</v>
       </c>
       <c r="C52" t="s" s="6">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D52" t="s" s="6">
         <v>21</v>
@@ -5880,7 +5865,7 @@
         <v>1.0229166666666667</v>
       </c>
       <c r="O52" t="s" s="9">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P52" t="n" s="11">
         <v>0.8854166666666666</v>
@@ -5909,7 +5894,7 @@
         <v>3.0</v>
       </c>
       <c r="C53" t="s" s="6">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D53" t="s" s="6">
         <v>21</v>
@@ -5945,7 +5930,7 @@
         <v>0.98125</v>
       </c>
       <c r="O53" t="s" s="9">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="P53" t="n" s="11">
         <v>0.9270833333333334</v>
@@ -5974,7 +5959,7 @@
         <v>3.0</v>
       </c>
       <c r="C54" t="s" s="6">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D54" t="s" s="6">
         <v>21</v>
@@ -6010,7 +5995,7 @@
         <v>0.9875</v>
       </c>
       <c r="O54" t="s" s="9">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="P54" t="n" s="11">
         <v>0.9194444444444444</v>
@@ -6039,7 +6024,7 @@
         <v>2.0</v>
       </c>
       <c r="C55" t="s" s="6">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D55" t="s" s="6">
         <v>21</v>
@@ -6104,7 +6089,7 @@
         <v>1.0</v>
       </c>
       <c r="C56" t="s" s="6">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D56" t="s" s="6">
         <v>21</v>
@@ -6140,7 +6125,7 @@
         <v>0.9909722222222223</v>
       </c>
       <c r="O56" t="s" s="9">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="P56" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -6169,7 +6154,7 @@
         <v>1.0</v>
       </c>
       <c r="C57" t="s" s="6">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D57" t="s" s="6">
         <v>21</v>
@@ -6214,7 +6199,7 @@
         <v>0.9548611111111112</v>
       </c>
       <c r="R57" t="s" s="9">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S57" t="n" s="11">
         <v>0.8923611111111112</v>
@@ -6234,7 +6219,7 @@
         <v>1.0</v>
       </c>
       <c r="C58" t="s" s="6">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D58" t="s" s="6">
         <v>21</v>
@@ -6270,7 +6255,7 @@
         <v>0.9895833333333334</v>
       </c>
       <c r="O58" t="s" s="9">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="P58" t="n" s="11">
         <v>0.9027777777777778</v>
@@ -6299,7 +6284,7 @@
         <v>1.0</v>
       </c>
       <c r="C59" t="s" s="6">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D59" t="s" s="6">
         <v>21</v>
@@ -6364,7 +6349,7 @@
         <v>3.0</v>
       </c>
       <c r="C60" t="s" s="6">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D60" t="s" s="6">
         <v>21</v>
@@ -6400,7 +6385,7 @@
         <v>0.9916666666666667</v>
       </c>
       <c r="O60" t="s" s="9">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="P60" t="n" s="11">
         <v>0.9083333333333333</v>
@@ -6429,7 +6414,7 @@
         <v>3.0</v>
       </c>
       <c r="C61" t="s" s="6">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D61" t="s" s="6">
         <v>21</v>
@@ -6465,7 +6450,7 @@
         <v>0.99375</v>
       </c>
       <c r="O61" t="s" s="9">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P61" t="n" s="11">
         <v>0.9055555555555556</v>
@@ -6494,7 +6479,7 @@
         <v>1.0</v>
       </c>
       <c r="C62" t="s" s="6">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D62" t="s" s="6">
         <v>21</v>
@@ -6530,7 +6515,7 @@
         <v>0.9659722222222222</v>
       </c>
       <c r="O62" t="s" s="9">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="P62" t="n" s="11">
         <v>0.8958333333333334</v>
@@ -6539,7 +6524,7 @@
         <v>0.9375</v>
       </c>
       <c r="R62" t="s" s="9">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="S62" t="n" s="11">
         <v>0.875</v>
@@ -6559,7 +6544,7 @@
         <v>3.0</v>
       </c>
       <c r="C63" t="s" s="6">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D63" t="s" s="6">
         <v>21</v>
@@ -6595,7 +6580,7 @@
         <v>0.9583333333333334</v>
       </c>
       <c r="O63" t="s" s="9">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="P63" t="n" s="11">
         <v>0.9125</v>
@@ -6624,7 +6609,7 @@
         <v>1.0</v>
       </c>
       <c r="C64" t="s" s="6">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D64" t="s" s="6">
         <v>21</v>
@@ -6660,7 +6645,7 @@
         <v>0.9368055555555556</v>
       </c>
       <c r="O64" t="s" s="9">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="P64" t="n" s="11">
         <v>0.8854166666666666</v>
@@ -6669,7 +6654,7 @@
         <v>0.9166666666666666</v>
       </c>
       <c r="R64" t="s" s="9">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S64" t="n" s="11">
         <v>0.8701388888888889</v>
@@ -6689,7 +6674,7 @@
         <v>3.0</v>
       </c>
       <c r="C65" t="s" s="6">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D65" t="s" s="6">
         <v>21</v>
@@ -6725,7 +6710,7 @@
         <v>0.9729166666666667</v>
       </c>
       <c r="O65" t="s" s="9">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="P65" t="n" s="11">
         <v>0.9215277777777777</v>
@@ -6754,7 +6739,7 @@
         <v>2.0</v>
       </c>
       <c r="C66" t="s" s="6">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D66" t="s" s="6">
         <v>21</v>
@@ -6790,7 +6775,7 @@
         <v>1.0027777777777778</v>
       </c>
       <c r="O66" t="s" s="9">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="P66" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -6819,7 +6804,7 @@
         <v>1.0</v>
       </c>
       <c r="C67" t="s" s="6">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D67" t="s" s="6">
         <v>21</v>
@@ -6884,7 +6869,7 @@
         <v>1.0</v>
       </c>
       <c r="C68" t="s" s="6">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D68" t="s" s="6">
         <v>21</v>
@@ -6920,7 +6905,7 @@
         <v>0.9791666666666666</v>
       </c>
       <c r="O68" t="s" s="9">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="P68" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -6929,7 +6914,7 @@
         <v>0.9381944444444444</v>
       </c>
       <c r="R68" t="s" s="9">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S68" t="n" s="11">
         <v>0.9277777777777778</v>
@@ -6949,7 +6934,7 @@
         <v>3.0</v>
       </c>
       <c r="C69" t="s" s="6">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D69" t="s" s="6">
         <v>21</v>
@@ -6985,7 +6970,7 @@
         <v>0.9680555555555556</v>
       </c>
       <c r="O69" t="s" s="9">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="P69" t="n" s="11">
         <v>0.9333333333333333</v>
@@ -7014,7 +6999,7 @@
         <v>3.0</v>
       </c>
       <c r="C70" t="s" s="6">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D70" t="s" s="6">
         <v>21</v>
@@ -7050,7 +7035,7 @@
         <v>0.9395833333333333</v>
       </c>
       <c r="O70" t="s" s="9">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="P70" t="n" s="11">
         <v>0.8541666666666666</v>
@@ -7059,7 +7044,7 @@
         <v>0.8958333333333334</v>
       </c>
       <c r="R70" t="s" s="9">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S70" t="n" s="11">
         <v>0.875</v>
@@ -7079,7 +7064,7 @@
         <v>3.0</v>
       </c>
       <c r="C71" t="s" s="6">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D71" t="s" s="6">
         <v>21</v>
@@ -7115,7 +7100,7 @@
         <v>0.9777777777777777</v>
       </c>
       <c r="O71" t="s" s="9">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P71" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -7124,7 +7109,7 @@
         <v>0.9513888888888888</v>
       </c>
       <c r="R71" t="s" s="9">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S71" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -7144,7 +7129,7 @@
         <v>3.0</v>
       </c>
       <c r="C72" t="s" s="6">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D72" t="s" s="6">
         <v>21</v>
@@ -7180,7 +7165,7 @@
         <v>0.9722222222222222</v>
       </c>
       <c r="O72" t="s" s="9">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="P72" t="n" s="11">
         <v>0.9097222222222222</v>
@@ -7209,7 +7194,7 @@
         <v>3.0</v>
       </c>
       <c r="C73" t="s" s="6">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D73" t="s" s="6">
         <v>21</v>
@@ -7245,7 +7230,7 @@
         <v>0.9715277777777778</v>
       </c>
       <c r="O73" t="s" s="9">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="P73" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -7274,7 +7259,7 @@
         <v>2.0</v>
       </c>
       <c r="C74" t="s" s="6">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D74" t="s" s="6">
         <v>21</v>
@@ -7310,7 +7295,7 @@
         <v>0.9673611111111111</v>
       </c>
       <c r="O74" t="s" s="9">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P74" t="n" s="11">
         <v>0.9361111111111111</v>
@@ -7339,7 +7324,7 @@
         <v>1.0</v>
       </c>
       <c r="C75" t="s" s="6">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D75" t="s" s="6">
         <v>21</v>
@@ -7404,7 +7389,7 @@
         <v>1.0</v>
       </c>
       <c r="C76" t="s" s="6">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D76" t="s" s="6">
         <v>21</v>
@@ -7440,7 +7425,7 @@
         <v>0.9319444444444445</v>
       </c>
       <c r="O76" t="s" s="9">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="P76" t="n" s="11">
         <v>0.8118055555555556</v>
@@ -7449,7 +7434,7 @@
         <v>0.8743055555555556</v>
       </c>
       <c r="R76" t="s" s="9">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="S76" t="n" s="11">
         <v>0.7805555555555556</v>
@@ -7469,7 +7454,7 @@
         <v>1.0</v>
       </c>
       <c r="C77" t="s" s="6">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D77" t="s" s="6">
         <v>21</v>
@@ -7534,7 +7519,7 @@
         <v>3.0</v>
       </c>
       <c r="C78" t="s" s="6">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D78" t="s" s="6">
         <v>21</v>
@@ -7570,7 +7555,7 @@
         <v>0.9944444444444445</v>
       </c>
       <c r="O78" t="s" s="9">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="P78" t="n" s="11">
         <v>0.9041666666666667</v>
@@ -7599,7 +7584,7 @@
         <v>2.0</v>
       </c>
       <c r="C79" t="s" s="6">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D79" t="s" s="6">
         <v>21</v>
@@ -7635,7 +7620,7 @@
         <v>0.9993055555555556</v>
       </c>
       <c r="O79" t="s" s="9">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P79" t="n" s="11">
         <v>0.8951388888888889</v>
@@ -7664,7 +7649,7 @@
         <v>2.0</v>
       </c>
       <c r="C80" t="s" s="6">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D80" t="s" s="6">
         <v>21</v>
@@ -7729,7 +7714,7 @@
         <v>2.0</v>
       </c>
       <c r="C81" t="s" s="6">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D81" t="s" s="6">
         <v>21</v>
@@ -7765,7 +7750,7 @@
         <v>0.9972222222222222</v>
       </c>
       <c r="O81" t="s" s="9">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="P81" t="n" s="11">
         <v>0.9111111111111111</v>
@@ -7794,7 +7779,7 @@
         <v>3.0</v>
       </c>
       <c r="C82" t="s" s="6">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D82" t="s" s="6">
         <v>21</v>
@@ -7830,7 +7815,7 @@
         <v>0.9722222222222222</v>
       </c>
       <c r="O82" t="s" s="9">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="P82" t="n" s="11">
         <v>0.9090277777777778</v>
@@ -7839,7 +7824,7 @@
         <v>0.9375</v>
       </c>
       <c r="R82" t="s" s="9">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="S82" t="n" s="11">
         <v>0.9083333333333333</v>
@@ -7859,7 +7844,7 @@
         <v>3.0</v>
       </c>
       <c r="C83" t="s" s="6">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D83" t="s" s="6">
         <v>21</v>
@@ -7895,7 +7880,7 @@
         <v>0.9930555555555556</v>
       </c>
       <c r="O83" t="s" s="9">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="P83" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -7924,7 +7909,7 @@
         <v>1.0</v>
       </c>
       <c r="C84" t="s" s="6">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D84" t="s" s="6">
         <v>21</v>
@@ -7960,7 +7945,7 @@
         <v>0.9826388888888888</v>
       </c>
       <c r="O84" t="s" s="9">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="P84" t="n" s="11">
         <v>0.9020833333333333</v>
@@ -7969,7 +7954,7 @@
         <v>0.9388888888888889</v>
       </c>
       <c r="R84" t="s" s="9">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="S84" t="n" s="11">
         <v>0.9111111111111111</v>
@@ -7989,7 +7974,7 @@
         <v>1.0</v>
       </c>
       <c r="C85" t="s" s="6">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D85" t="s" s="6">
         <v>21</v>
@@ -8054,7 +8039,7 @@
         <v>2.0</v>
       </c>
       <c r="C86" t="s" s="6">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D86" t="s" s="6">
         <v>21</v>
@@ -8090,7 +8075,7 @@
         <v>0.975</v>
       </c>
       <c r="O86" t="s" s="9">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="P86" t="n" s="11">
         <v>0.9173611111111111</v>
@@ -8099,7 +8084,7 @@
         <v>0.9409722222222222</v>
       </c>
       <c r="R86" t="s" s="9">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="S86" t="n" s="11">
         <v>0.9173611111111111</v>
@@ -8119,7 +8104,7 @@
         <v>2.0</v>
       </c>
       <c r="C87" t="s" s="6">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D87" t="s" s="6">
         <v>21</v>
@@ -8155,7 +8140,7 @@
         <v>1.0055555555555555</v>
       </c>
       <c r="O87" t="s" s="9">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P87" t="n" s="11">
         <v>0.8965277777777778</v>
@@ -8184,7 +8169,7 @@
         <v>3.0</v>
       </c>
       <c r="C88" t="s" s="6">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D88" t="s" s="6">
         <v>21</v>
@@ -8220,7 +8205,7 @@
         <v>0.9784722222222222</v>
       </c>
       <c r="O88" t="s" s="9">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="P88" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -8307,9 +8292,7 @@
       <c r="B90" t="n" s="6">
         <v>1.0</v>
       </c>
-      <c r="C90" t="s" s="6">
-        <v>193</v>
-      </c>
+      <c r="C90" s="6"/>
       <c r="D90" t="s" s="6">
         <v>21</v>
       </c>
@@ -8343,18 +8326,14 @@
       <c r="N90" t="n" s="11">
         <v>1.0215277777777778</v>
       </c>
-      <c r="O90" t="s" s="9">
-        <v>194</v>
-      </c>
+      <c r="O90" s="9"/>
       <c r="P90" t="n" s="11">
         <v>0.9055555555555556</v>
       </c>
       <c r="Q90" t="n" s="11">
         <v>0.9416666666666667</v>
       </c>
-      <c r="R90" t="s" s="9">
-        <v>26</v>
-      </c>
+      <c r="R90" s="9"/>
       <c r="S90" t="n" s="11">
         <v>0.9145833333333333</v>
       </c>
@@ -8373,7 +8352,7 @@
         <v>1.0</v>
       </c>
       <c r="C91" t="s" s="6">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D91" t="s" s="6">
         <v>21</v>
@@ -8409,7 +8388,7 @@
         <v>0.98125</v>
       </c>
       <c r="O91" t="s" s="9">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="P91" t="n" s="11">
         <v>0.9020833333333333</v>
@@ -8438,7 +8417,7 @@
         <v>3.0</v>
       </c>
       <c r="C92" t="s" s="6">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D92" t="s" s="6">
         <v>21</v>
@@ -8474,7 +8453,7 @@
         <v>0.9527777777777777</v>
       </c>
       <c r="O92" t="s" s="9">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="P92" t="n" s="11">
         <v>0.8993055555555556</v>
@@ -8502,7 +8481,9 @@
       <c r="B93" t="n" s="6">
         <v>3.0</v>
       </c>
-      <c r="C93" s="6"/>
+      <c r="C93" t="s" s="6">
+        <v>195</v>
+      </c>
       <c r="D93" t="s" s="6">
         <v>21</v>
       </c>
@@ -8536,14 +8517,18 @@
       <c r="N93" t="n" s="11">
         <v>1.0034722222222223</v>
       </c>
-      <c r="O93" s="9"/>
+      <c r="O93" t="s" s="9">
+        <v>26</v>
+      </c>
       <c r="P93" t="n" s="11">
         <v>0.8756944444444444</v>
       </c>
       <c r="Q93" t="n" s="11">
         <v>0.9104166666666667</v>
       </c>
-      <c r="R93" s="9"/>
+      <c r="R93" t="s" s="9">
+        <v>196</v>
+      </c>
       <c r="S93" t="n" s="11">
         <v>0.9027777777777778</v>
       </c>
@@ -8562,7 +8547,7 @@
         <v>3.0</v>
       </c>
       <c r="C94" t="s" s="6">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D94" t="s" s="6">
         <v>21</v>
@@ -8627,7 +8612,7 @@
         <v>3.0</v>
       </c>
       <c r="C95" t="s" s="6">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D95" t="s" s="6">
         <v>21</v>
@@ -8663,7 +8648,7 @@
         <v>0.9930555555555556</v>
       </c>
       <c r="O95" t="s" s="9">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="P95" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -8692,7 +8677,7 @@
         <v>3.0</v>
       </c>
       <c r="C96" t="s" s="6">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D96" t="s" s="6">
         <v>21</v>
@@ -8757,7 +8742,7 @@
         <v>3.0</v>
       </c>
       <c r="C97" t="s" s="6">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D97" t="s" s="6">
         <v>21</v>
@@ -8793,7 +8778,7 @@
         <v>0.9722222222222222</v>
       </c>
       <c r="O97" t="s" s="9">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="P97" t="n" s="11">
         <v>0.9166666666666666</v>
@@ -8822,7 +8807,7 @@
         <v>1.0</v>
       </c>
       <c r="C98" t="s" s="6">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D98" t="s" s="6">
         <v>21</v>
@@ -8858,7 +8843,7 @@
         <v>0.9743055555555555</v>
       </c>
       <c r="O98" t="s" s="9">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="P98" t="n" s="11">
         <v>0.89375</v>
@@ -8887,7 +8872,7 @@
         <v>3.0</v>
       </c>
       <c r="C99" t="s" s="6">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D99" t="s" s="6">
         <v>21</v>
@@ -8952,7 +8937,7 @@
         <v>1.0</v>
       </c>
       <c r="C100" t="s" s="6">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D100" t="s" s="6">
         <v>21</v>
@@ -8988,7 +8973,7 @@
         <v>0.9618055555555556</v>
       </c>
       <c r="O100" t="s" s="9">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="P100" t="n" s="11">
         <v>0.8993055555555556</v>
@@ -9017,7 +9002,7 @@
         <v>3.0</v>
       </c>
       <c r="C101" t="s" s="6">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D101" t="s" s="6">
         <v>21</v>
@@ -9053,7 +9038,7 @@
         <v>0.9902777777777778</v>
       </c>
       <c r="O101" t="s" s="9">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="P101" t="n" s="11">
         <v>0.9131944444444444</v>
@@ -9062,7 +9047,7 @@
         <v>0.9291666666666667</v>
       </c>
       <c r="R101" t="s" s="9">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="S101" t="n" s="11">
         <v>0.9368055555555556</v>
@@ -9082,7 +9067,7 @@
         <v>2.0</v>
       </c>
       <c r="C102" t="s" s="6">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D102" t="s" s="6">
         <v>21</v>
@@ -9147,7 +9132,7 @@
         <v>2.0</v>
       </c>
       <c r="C103" t="s" s="6">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D103" t="s" s="6">
         <v>21</v>
@@ -9183,7 +9168,7 @@
         <v>1.0347222222222223</v>
       </c>
       <c r="O103" t="s" s="9">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P103" t="n" s="11">
         <v>0.9354166666666667</v>
@@ -9212,7 +9197,7 @@
         <v>2.0</v>
       </c>
       <c r="C104" t="s" s="6">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D104" t="s" s="6">
         <v>21</v>
@@ -9257,7 +9242,7 @@
         <v>0.9444444444444444</v>
       </c>
       <c r="R104" t="s" s="9">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S104" t="n" s="11">
         <v>0.9236111111111112</v>
@@ -9277,7 +9262,7 @@
         <v>2.0</v>
       </c>
       <c r="C105" t="s" s="6">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D105" t="s" s="6">
         <v>21</v>
@@ -9313,7 +9298,7 @@
         <v>1.0048611111111112</v>
       </c>
       <c r="O105" t="s" s="9">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="P105" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9342,7 +9327,7 @@
         <v>1.0</v>
       </c>
       <c r="C106" t="s" s="6">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D106" t="s" s="6">
         <v>21</v>
@@ -9407,7 +9392,7 @@
         <v>2.0</v>
       </c>
       <c r="C107" t="s" s="6">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D107" t="s" s="6">
         <v>21</v>
@@ -9470,7 +9455,7 @@
         <v>2.0</v>
       </c>
       <c r="C108" t="s" s="6">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D108" t="s" s="6">
         <v>21</v>
@@ -9515,7 +9500,7 @@
         <v>0.9395833333333333</v>
       </c>
       <c r="R108" t="s" s="9">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S108" t="n" s="11">
         <v>0.9340277777777778</v>
@@ -9535,7 +9520,7 @@
         <v>2.0</v>
       </c>
       <c r="C109" t="s" s="6">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D109" t="s" s="6">
         <v>21</v>
@@ -9580,7 +9565,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R109" t="s" s="9">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="S109" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9600,7 +9585,7 @@
         <v>2.0</v>
       </c>
       <c r="C110" t="s" s="6">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D110" t="s" s="6">
         <v>21</v>
@@ -9636,7 +9621,7 @@
         <v>1.0256944444444445</v>
       </c>
       <c r="O110" t="s" s="9">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P110" t="n" s="11">
         <v>0.9305555555555556</v>
@@ -9665,7 +9650,7 @@
         <v>2.0</v>
       </c>
       <c r="C111" t="s" s="6">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D111" t="s" s="6">
         <v>21</v>
@@ -9701,7 +9686,7 @@
         <v>1.0208333333333333</v>
       </c>
       <c r="O111" t="s" s="9">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="P111" t="n" s="11">
         <v>0.9326388888888889</v>
@@ -9710,7 +9695,7 @@
         <v>0.9416666666666667</v>
       </c>
       <c r="R111" t="s" s="9">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="S111" t="n" s="11">
         <v>0.9326388888888889</v>
@@ -9730,7 +9715,7 @@
         <v>3.0</v>
       </c>
       <c r="C112" t="s" s="6">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D112" t="s" s="6">
         <v>21</v>
@@ -9766,7 +9751,7 @@
         <v>0.99375</v>
       </c>
       <c r="O112" t="s" s="9">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="P112" t="n" s="11">
         <v>0.9263888888888889</v>
@@ -9795,7 +9780,7 @@
         <v>1.0</v>
       </c>
       <c r="C113" t="s" s="6">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D113" t="s" s="6">
         <v>21</v>
@@ -9831,7 +9816,7 @@
         <v>0.9986111111111111</v>
       </c>
       <c r="O113" t="s" s="9">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="P113" t="n" s="11">
         <v>0.9333333333333333</v>
@@ -9860,7 +9845,7 @@
         <v>2.0</v>
       </c>
       <c r="C114" t="s" s="6">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D114" t="s" s="6">
         <v>21</v>
@@ -9894,7 +9879,7 @@
         <v>0.9875</v>
       </c>
       <c r="O114" t="s" s="9">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="P114" t="n" s="11">
         <v>0.9333333333333333</v>
@@ -9923,7 +9908,7 @@
         <v>2.0</v>
       </c>
       <c r="C115" t="s" s="6">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D115" t="s" s="6">
         <v>21</v>
@@ -9957,7 +9942,7 @@
         <v>0.9861111111111112</v>
       </c>
       <c r="O115" t="s" s="9">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="P115" t="n" s="11">
         <v>0.9298611111111111</v>

</xml_diff>